<commit_message>
add the data for the fish with 6 observations
</commit_message>
<xml_diff>
--- a/fish-weights.xlsx
+++ b/fish-weights.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/au690221/work/teaching/aarhus/courses/dyr-og-data/course/w01-1/activities/80-dyr-og-væv-repo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/au690221/work/teaching/aarhus/courses/dyr-og-data/course/w01-1/activities/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{514CA48E-6F83-8046-824C-F91F74009839}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90A07FE9-D568-884F-886C-206C65ACC01B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3080" yWindow="2060" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{21EC0220-5DA7-3849-B2A2-C6C16413E8D0}"/>
+    <workbookView xWindow="3080" yWindow="2060" windowWidth="28040" windowHeight="17440" xr2:uid="{21EC0220-5DA7-3849-B2A2-C6C16413E8D0}"/>
   </bookViews>
   <sheets>
     <sheet name="fish-meta" sheetId="1" r:id="rId1"/>
@@ -429,7 +429,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F62EC19-7439-4F46-845D-71346F7A26D4}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
@@ -655,10 +655,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E066650-3DBC-B94E-A5A3-F6FCA92DB12B}">
-  <dimension ref="A1:B43"/>
+  <dimension ref="A1:B66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -697,313 +697,497 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="B5">
-        <v>0.30930000000000002</v>
+        <v>0.32900000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="B6">
-        <v>0.30630000000000002</v>
+        <v>0.3301</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="B7">
-        <v>0.30599999999999999</v>
+        <v>0.32950000000000002</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B8">
-        <v>0.47470000000000001</v>
+        <v>0.30930000000000002</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B9">
-        <v>0.44850000000000001</v>
+        <v>0.30630000000000002</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B10">
-        <v>0.44740000000000002</v>
+        <v>0.30599999999999999</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B11">
-        <v>0.48549999999999999</v>
+        <v>0.47470000000000001</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B12">
-        <v>0.44790000000000002</v>
+        <v>0.44850000000000001</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B13">
-        <v>0.44479999999999997</v>
+        <v>0.44740000000000002</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B14">
-        <v>0.56950000000000001</v>
+        <v>0.48549999999999999</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B15">
-        <v>0.55910000000000004</v>
+        <v>0.44790000000000002</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B16">
-        <v>0.56220000000000003</v>
+        <v>0.44479999999999997</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B17">
-        <v>0.3826</v>
+        <v>0.4788</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B18">
-        <v>0.36919999999999997</v>
+        <v>0.4602</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B19">
-        <v>0.36980000000000002</v>
+        <v>0.44350000000000001</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B20">
-        <v>0.65549999999999997</v>
+        <v>0.56950000000000001</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B21">
-        <v>0.66590000000000005</v>
+        <v>0.55910000000000004</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B22">
-        <v>0.65449999999999997</v>
+        <v>0.56220000000000003</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B23">
-        <v>0.55900000000000005</v>
+        <v>0.3826</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B24">
-        <v>0.54200000000000004</v>
+        <v>0.36919999999999997</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B25">
-        <v>0.54310000000000003</v>
+        <v>0.36980000000000002</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B26">
-        <v>0.37919999999999998</v>
+        <v>0.65549999999999997</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B27">
-        <v>0.37569999999999998</v>
+        <v>0.66590000000000005</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B28">
-        <v>0.36859999999999998</v>
+        <v>0.65449999999999997</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B29">
-        <v>0.46500000000000002</v>
+        <v>0.55900000000000005</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B30">
-        <v>0.4577</v>
+        <v>0.54200000000000004</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B31">
-        <v>0.4536</v>
+        <v>0.54310000000000003</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="B32">
-        <v>0.31509999999999999</v>
+        <v>0.53169999999999995</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="B33">
-        <v>0.3029</v>
+        <v>0.52390000000000003</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="B34">
-        <v>0.2969</v>
+        <v>0.51880000000000004</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B35">
-        <v>0.56259999999999999</v>
+        <v>0.37919999999999998</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B36">
-        <v>0.56920000000000004</v>
+        <v>0.37569999999999998</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B37">
-        <v>0.56440000000000001</v>
+        <v>0.36859999999999998</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B38">
-        <v>0.52</v>
+        <v>0.36720000000000003</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B39">
-        <v>0.51</v>
+        <v>0.35610000000000003</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B40">
-        <v>0.52</v>
+        <v>0.35320000000000001</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B41">
-        <v>0.64039999999999997</v>
+        <v>0.46500000000000002</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B42">
-        <v>0.64100000000000001</v>
+        <v>0.4577</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43">
+        <v>8</v>
+      </c>
+      <c r="B43">
+        <v>0.4536</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>8</v>
+      </c>
+      <c r="B44">
+        <v>0.45290000000000002</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>8</v>
+      </c>
+      <c r="B45">
+        <v>0.45369999999999999</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>8</v>
+      </c>
+      <c r="B46">
+        <v>0.44940000000000002</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>2</v>
+      </c>
+      <c r="B47">
+        <v>0.31509999999999999</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>2</v>
+      </c>
+      <c r="B48">
+        <v>0.3029</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>2</v>
+      </c>
+      <c r="B49">
+        <v>0.2969</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>2</v>
+      </c>
+      <c r="B50">
+        <v>0.29749999999999999</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>2</v>
+      </c>
+      <c r="B51">
+        <v>0.28549999999999998</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>2</v>
+      </c>
+      <c r="B52">
+        <v>0.28299999999999997</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>11</v>
+      </c>
+      <c r="B53">
+        <v>0.56259999999999999</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>11</v>
+      </c>
+      <c r="B54">
+        <v>0.56920000000000004</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>11</v>
+      </c>
+      <c r="B55">
+        <v>0.56440000000000001</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>11</v>
+      </c>
+      <c r="B56">
+        <v>0.55989999999999995</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>11</v>
+      </c>
+      <c r="B57">
+        <v>0.5484</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>12</v>
+      </c>
+      <c r="B58">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>12</v>
+      </c>
+      <c r="B59">
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>12</v>
+      </c>
+      <c r="B60">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>12</v>
+      </c>
+      <c r="B61">
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>12</v>
+      </c>
+      <c r="B62">
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>12</v>
+      </c>
+      <c r="B63">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64">
         <v>7</v>
       </c>
-      <c r="B43">
+      <c r="B64">
+        <v>0.64039999999999997</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>7</v>
+      </c>
+      <c r="B65">
+        <v>0.64100000000000001</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>7</v>
+      </c>
+      <c r="B66">
         <v>0.61990000000000001</v>
       </c>
     </row>

</xml_diff>